<commit_message>
add link to wq report card in text for wq content
</commit_message>
<xml_diff>
--- a/data-raw/swfwmdrainfall.xlsx
+++ b/data-raw/swfwmdrainfall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swfwmd-my.sharepoint.com/personal/erin_walters_swfwmd_state_fl_us/Documents/DECRain/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swfwmd-my.sharepoint.com/personal/erin_walters_swfwmd_state_fl_us/Documents/JANRain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7ACEC942-7F4D-449A-8841-4606B4D19748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92873990-28F5-4CB6-960E-22B661269E2E}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{7ACEC942-7F4D-449A-8841-4606B4D19748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{400520CA-8F0E-4348-AD2A-2DB84DA0B2A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-435" windowWidth="29040" windowHeight="15720" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jan-usgsbsn" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,13 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="17" state="veryHidden" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="ann_usgsbasin" localSheetId="12">'ann-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="ann_usgsbasin" localSheetId="12">'ann-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="apr_usgsbasin" localSheetId="3">'apr-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="aug_usgsbasin" localSheetId="7">'aug-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="dec_usgsbasin" localSheetId="11">'dec-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="dry_usgsbasin" localSheetId="14">'dry-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="feb_usgsbasin" localSheetId="1">'feb-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="jan_usgsbasin" localSheetId="0">'jan-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="jan_usgsbasin" localSheetId="0">'jan-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="jul_usgsbasin" localSheetId="6">'jul-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="jun_usgsbasin" localSheetId="5">'jun-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="mar_usgsbasin" localSheetId="2">'mar-usgsbsn'!$A$1:$N$115</definedName>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="34">
   <si>
     <t>January Rainfall Summary Data by USGS Drainage Basin</t>
   </si>
@@ -1033,7 +1033,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -6041,134 +6041,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>0.06</v>
+        <v>3.02</v>
       </c>
       <c r="C113" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0</v>
+        <v>1.94</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>0.03</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="F113" s="3">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="G113" s="3">
-        <v>0</v>
+        <v>2.09</v>
       </c>
       <c r="H113" s="3">
-        <v>0.03</v>
+        <v>1.64</v>
       </c>
       <c r="I113" s="3">
-        <v>0.06</v>
+        <v>1.75</v>
       </c>
       <c r="J113" s="3">
-        <v>0.05</v>
+        <v>1.46</v>
       </c>
       <c r="K113" s="3">
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="L113" s="3">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="M113" s="3">
-        <v>0</v>
+        <v>1.51</v>
       </c>
       <c r="N113" s="3">
-        <v>0</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>3.02</v>
+        <v>0.06</v>
       </c>
       <c r="C114" s="3">
-        <v>2.62</v>
+        <v>0.02</v>
       </c>
       <c r="D114" s="3">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="E114" s="3">
-        <v>2.5299999999999998</v>
+        <v>0.03</v>
       </c>
       <c r="F114" s="3">
-        <v>2.15</v>
+        <v>0</v>
       </c>
       <c r="G114" s="3">
-        <v>2.42</v>
+        <v>0</v>
       </c>
       <c r="H114" s="3">
-        <v>2.16</v>
+        <v>0.03</v>
       </c>
       <c r="I114" s="3">
-        <v>2.4</v>
+        <v>0.06</v>
       </c>
       <c r="J114" s="3">
-        <v>2.4300000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="K114" s="3">
-        <v>2.42</v>
+        <v>0</v>
       </c>
       <c r="L114" s="3">
-        <v>2.33</v>
+        <v>0</v>
       </c>
       <c r="M114" s="3">
-        <v>2.21</v>
+        <v>0</v>
       </c>
       <c r="N114" s="3">
-        <v>2.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>3.02</v>
+      </c>
+      <c r="C115" s="3">
+        <v>2.61</v>
+      </c>
+      <c r="D115" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E115" s="3">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F115" s="3">
+        <v>2.14</v>
+      </c>
+      <c r="G115" s="3">
+        <v>2.42</v>
+      </c>
+      <c r="H115" s="3">
+        <v>2.15</v>
+      </c>
+      <c r="I115" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="J115" s="3">
+        <v>2.42</v>
+      </c>
+      <c r="K115" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="L115" s="3">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="M115" s="3">
+        <v>2.21</v>
+      </c>
+      <c r="N115" s="3">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>10.76</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>7.39</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>7.45</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>7.52</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>7.57</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>8.0299999999999994</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>7.69</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>7.99</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>8.02</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>8.08</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>8.64</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>7.63</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>10.51</v>
       </c>
     </row>
@@ -21809,7 +21853,7 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -26817,134 +26861,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B113" s="3">
-        <v>31.96</v>
-      </c>
-      <c r="C113" s="3">
-        <v>32.08</v>
-      </c>
-      <c r="D113" s="3">
-        <v>37.840000000000003</v>
-      </c>
-      <c r="E113" s="3">
-        <v>31.42</v>
-      </c>
-      <c r="F113" s="3">
-        <v>28.75</v>
-      </c>
-      <c r="G113" s="3">
-        <v>33.43</v>
-      </c>
-      <c r="H113" s="3">
-        <v>30.72</v>
-      </c>
-      <c r="I113" s="3">
-        <v>33.229999999999997</v>
-      </c>
-      <c r="J113" s="3">
-        <v>35.25</v>
-      </c>
-      <c r="K113" s="3">
-        <v>31.66</v>
-      </c>
-      <c r="L113" s="3">
-        <v>30.19</v>
-      </c>
-      <c r="M113" s="3">
-        <v>37.24</v>
-      </c>
-      <c r="N113" s="3">
-        <v>30.03</v>
+      <c r="A113" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N113" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>54.12</v>
+        <v>31.96</v>
       </c>
       <c r="C114" s="3">
-        <v>52.96</v>
+        <v>32.08</v>
       </c>
       <c r="D114" s="3">
-        <v>54.37</v>
+        <v>37.840000000000003</v>
       </c>
       <c r="E114" s="3">
-        <v>53.78</v>
+        <v>31.42</v>
       </c>
       <c r="F114" s="3">
-        <v>51.94</v>
+        <v>28.75</v>
       </c>
       <c r="G114" s="3">
-        <v>51.75</v>
+        <v>33.43</v>
       </c>
       <c r="H114" s="3">
-        <v>52.12</v>
+        <v>30.72</v>
       </c>
       <c r="I114" s="3">
-        <v>52.61</v>
+        <v>33.229999999999997</v>
       </c>
       <c r="J114" s="3">
-        <v>52.93</v>
+        <v>35.25</v>
       </c>
       <c r="K114" s="3">
-        <v>53.52</v>
+        <v>31.66</v>
       </c>
       <c r="L114" s="3">
-        <v>51.74</v>
+        <v>30.19</v>
       </c>
       <c r="M114" s="3">
-        <v>53.23</v>
+        <v>37.24</v>
       </c>
       <c r="N114" s="3">
-        <v>51.34</v>
+        <v>30.03</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>54.12</v>
+      </c>
+      <c r="C115" s="3">
+        <v>52.96</v>
+      </c>
+      <c r="D115" s="3">
+        <v>54.37</v>
+      </c>
+      <c r="E115" s="3">
+        <v>53.78</v>
+      </c>
+      <c r="F115" s="3">
+        <v>51.94</v>
+      </c>
+      <c r="G115" s="3">
+        <v>51.75</v>
+      </c>
+      <c r="H115" s="3">
+        <v>52.12</v>
+      </c>
+      <c r="I115" s="3">
+        <v>52.61</v>
+      </c>
+      <c r="J115" s="3">
+        <v>52.93</v>
+      </c>
+      <c r="K115" s="3">
+        <v>53.52</v>
+      </c>
+      <c r="L115" s="3">
+        <v>51.74</v>
+      </c>
+      <c r="M115" s="3">
+        <v>53.23</v>
+      </c>
+      <c r="N115" s="3">
+        <v>51.34</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>78.72</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>76.819999999999993</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>78.38</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>77.66</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>75.88</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>82.14</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>77.849999999999994</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>77.78</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>81.45</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>87.44</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>85.54</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>80.41</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>88.1</v>
       </c>
     </row>
@@ -37211,43 +37299,43 @@
         <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>7.84</v>
+        <v>10.86</v>
       </c>
       <c r="C113" s="3">
-        <v>12</v>
+        <v>13.94</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>15.55</v>
+        <v>17.87</v>
       </c>
       <c r="F113" s="3">
-        <v>7.9</v>
+        <v>9.59</v>
       </c>
       <c r="G113" s="3">
-        <v>15.42</v>
+        <v>17.510000000000002</v>
       </c>
       <c r="H113" s="3">
-        <v>7.54</v>
+        <v>9.18</v>
       </c>
       <c r="I113" s="3">
-        <v>10.25</v>
+        <v>12</v>
       </c>
       <c r="J113" s="3">
-        <v>9.85</v>
+        <v>11.31</v>
       </c>
       <c r="K113" s="3">
-        <v>8.73</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="L113" s="3">
-        <v>9.33</v>
+        <v>10.45</v>
       </c>
       <c r="M113" s="3">
-        <v>8.43</v>
+        <v>9.94</v>
       </c>
       <c r="N113" s="3">
-        <v>7.94</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
@@ -37255,7 +37343,7 @@
         <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>7.84</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="C114" s="3">
         <v>10.92</v>
@@ -37267,22 +37355,22 @@
         <v>10.29</v>
       </c>
       <c r="F114" s="3">
-        <v>7.9</v>
+        <v>9.16</v>
       </c>
       <c r="G114" s="3">
         <v>9.0399999999999991</v>
       </c>
       <c r="H114" s="3">
-        <v>7.54</v>
+        <v>9.18</v>
       </c>
       <c r="I114" s="3">
-        <v>10.25</v>
+        <v>10.46</v>
       </c>
       <c r="J114" s="3">
         <v>9.5399999999999991</v>
       </c>
       <c r="K114" s="3">
-        <v>8.73</v>
+        <v>9.31</v>
       </c>
       <c r="L114" s="3">
         <v>7.85</v>
@@ -37299,43 +37387,43 @@
         <v>16</v>
       </c>
       <c r="B115" s="3">
-        <v>24.46</v>
+        <v>24.48</v>
       </c>
       <c r="C115" s="3">
-        <v>22.8</v>
+        <v>22.82</v>
       </c>
       <c r="D115" s="3">
         <v>22.99</v>
       </c>
       <c r="E115" s="3">
-        <v>22.28</v>
+        <v>22.31</v>
       </c>
       <c r="F115" s="3">
-        <v>20.92</v>
+        <v>20.94</v>
       </c>
       <c r="G115" s="3">
-        <v>20.68</v>
+        <v>20.7</v>
       </c>
       <c r="H115" s="3">
-        <v>20.43</v>
+        <v>20.45</v>
       </c>
       <c r="I115" s="3">
-        <v>21.32</v>
+        <v>21.33</v>
       </c>
       <c r="J115" s="3">
-        <v>20.85</v>
+        <v>20.86</v>
       </c>
       <c r="K115" s="3">
-        <v>20.43</v>
+        <v>20.440000000000001</v>
       </c>
       <c r="L115" s="3">
-        <v>20.079999999999998</v>
+        <v>20.09</v>
       </c>
       <c r="M115" s="3">
-        <v>19.989999999999998</v>
+        <v>20.010000000000002</v>
       </c>
       <c r="N115" s="3">
-        <v>19.27</v>
+        <v>19.28</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
rainfall plot as 20 year mean
</commit_message>
<xml_diff>
--- a/data-raw/swfwmdrainfall.xlsx
+++ b/data-raw/swfwmdrainfall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swfwmd-my.sharepoint.com/personal/erin_walters_swfwmd_state_fl_us/Documents/JANRain/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swfwmd-my.sharepoint.com/personal/erin_walters_swfwmd_state_fl_us/Documents/Mar25Rain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{7ACEC942-7F4D-449A-8841-4606B4D19748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{400520CA-8F0E-4348-AD2A-2DB84DA0B2A3}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{7ACEC942-7F4D-449A-8841-4606B4D19748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C38F2A38-7297-4D2C-B3BF-4B6B54C0E48D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-435" windowWidth="29040" windowHeight="15720" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jan-usgsbsn" sheetId="1" r:id="rId1"/>
@@ -37,11 +37,11 @@
     <definedName name="aug_usgsbasin" localSheetId="7">'aug-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="dec_usgsbasin" localSheetId="11">'dec-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="dry_usgsbasin" localSheetId="14">'dry-usgsbsn'!$A$1:$N$116</definedName>
-    <definedName name="feb_usgsbasin" localSheetId="1">'feb-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="feb_usgsbasin" localSheetId="1">'feb-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="jan_usgsbasin" localSheetId="0">'jan-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="jul_usgsbasin" localSheetId="6">'jul-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="jun_usgsbasin" localSheetId="5">'jun-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="mar_usgsbasin" localSheetId="2">'mar-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="mar_usgsbasin" localSheetId="2">'mar-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="may_usgsbasin" localSheetId="4">'may-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="nov_usgsbasin" localSheetId="10">'nov-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="oct_usgsbasin" localSheetId="9">'oct-usgsbsn'!$A$1:$N$115</definedName>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="34">
   <si>
     <t>January Rainfall Summary Data by USGS Drainage Basin</t>
   </si>
@@ -1039,23 +1039,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="44.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6233,23 +6233,23 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="45" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -11379,23 +11379,23 @@
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -16619,23 +16619,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -21859,23 +21859,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="53.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -27052,23 +27052,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="63.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -32200,23 +32200,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="59.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -37299,43 +37299,43 @@
         <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>10.86</v>
+        <v>15.51</v>
       </c>
       <c r="C113" s="3">
-        <v>13.94</v>
+        <v>17.14</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>17.87</v>
+        <v>21.36</v>
       </c>
       <c r="F113" s="3">
-        <v>9.59</v>
+        <v>13.42</v>
       </c>
       <c r="G113" s="3">
-        <v>17.510000000000002</v>
+        <v>21.18</v>
       </c>
       <c r="H113" s="3">
-        <v>9.18</v>
+        <v>12.17</v>
       </c>
       <c r="I113" s="3">
-        <v>12</v>
+        <v>15.2</v>
       </c>
       <c r="J113" s="3">
-        <v>11.31</v>
+        <v>14.05</v>
       </c>
       <c r="K113" s="3">
-        <v>9.8000000000000007</v>
+        <v>12.61</v>
       </c>
       <c r="L113" s="3">
-        <v>10.45</v>
+        <v>13.24</v>
       </c>
       <c r="M113" s="3">
-        <v>9.94</v>
+        <v>12.86</v>
       </c>
       <c r="N113" s="3">
-        <v>9.4</v>
+        <v>12.16</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
@@ -37361,7 +37361,7 @@
         <v>9.0399999999999991</v>
       </c>
       <c r="H114" s="3">
-        <v>9.18</v>
+        <v>9.82</v>
       </c>
       <c r="I114" s="3">
         <v>10.46</v>
@@ -37387,43 +37387,43 @@
         <v>16</v>
       </c>
       <c r="B115" s="3">
-        <v>24.48</v>
+        <v>24.52</v>
       </c>
       <c r="C115" s="3">
-        <v>22.82</v>
+        <v>22.85</v>
       </c>
       <c r="D115" s="3">
         <v>22.99</v>
       </c>
       <c r="E115" s="3">
-        <v>22.31</v>
+        <v>22.34</v>
       </c>
       <c r="F115" s="3">
-        <v>20.94</v>
+        <v>20.97</v>
       </c>
       <c r="G115" s="3">
-        <v>20.7</v>
+        <v>20.73</v>
       </c>
       <c r="H115" s="3">
-        <v>20.45</v>
+        <v>20.48</v>
       </c>
       <c r="I115" s="3">
-        <v>21.33</v>
+        <v>21.36</v>
       </c>
       <c r="J115" s="3">
-        <v>20.86</v>
+        <v>20.89</v>
       </c>
       <c r="K115" s="3">
-        <v>20.440000000000001</v>
+        <v>20.46</v>
       </c>
       <c r="L115" s="3">
-        <v>20.09</v>
+        <v>20.12</v>
       </c>
       <c r="M115" s="3">
-        <v>20.010000000000002</v>
+        <v>20.03</v>
       </c>
       <c r="N115" s="3">
-        <v>19.28</v>
+        <v>19.309999999999999</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -37486,23 +37486,23 @@
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="65.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -42786,7 +42786,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -42796,29 +42796,29 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="6.44140625" style="1"/>
+    <col min="1" max="1" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="6.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -47804,134 +47804,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>0.48</v>
+        <v>1.28</v>
       </c>
       <c r="C113" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0.4</v>
+        <v>1.23</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>0.23</v>
+        <v>2.02</v>
       </c>
       <c r="F113" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="G113" s="3">
-        <v>0.12</v>
+        <v>2.09</v>
       </c>
       <c r="H113" s="3">
-        <v>0.09</v>
+        <v>2</v>
       </c>
       <c r="I113" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>2.59</v>
       </c>
       <c r="J113" s="3">
-        <v>0.04</v>
+        <v>2.1</v>
       </c>
       <c r="K113" s="3">
-        <v>0.02</v>
+        <v>2.25</v>
       </c>
       <c r="L113" s="3">
-        <v>0.02</v>
+        <v>1.87</v>
       </c>
       <c r="M113" s="3">
-        <v>0.01</v>
+        <v>1.55</v>
       </c>
       <c r="N113" s="3">
-        <v>0</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>3.22</v>
+        <v>0.48</v>
       </c>
       <c r="C114" s="3">
-        <v>2.84</v>
+        <v>0.26</v>
       </c>
       <c r="D114" s="3">
-        <v>2.99</v>
+        <v>0.4</v>
       </c>
       <c r="E114" s="3">
-        <v>2.84</v>
+        <v>0.23</v>
       </c>
       <c r="F114" s="3">
-        <v>2.4700000000000002</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G114" s="3">
-        <v>2.74</v>
+        <v>0.12</v>
       </c>
       <c r="H114" s="3">
-        <v>2.4300000000000002</v>
+        <v>0.09</v>
       </c>
       <c r="I114" s="3">
-        <v>2.73</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J114" s="3">
-        <v>2.72</v>
+        <v>0.04</v>
       </c>
       <c r="K114" s="3">
-        <v>2.68</v>
+        <v>0.02</v>
       </c>
       <c r="L114" s="3">
-        <v>2.52</v>
+        <v>0.02</v>
       </c>
       <c r="M114" s="3">
-        <v>2.4500000000000002</v>
+        <v>0.01</v>
       </c>
       <c r="N114" s="3">
-        <v>2.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>3.21</v>
+      </c>
+      <c r="C115" s="3">
+        <v>2.83</v>
+      </c>
+      <c r="D115" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="E115" s="3">
+        <v>2.83</v>
+      </c>
+      <c r="F115" s="3">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G115" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="H115" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I115" s="3">
+        <v>2.73</v>
+      </c>
+      <c r="J115" s="3">
+        <v>2.72</v>
+      </c>
+      <c r="K115" s="3">
+        <v>2.67</v>
+      </c>
+      <c r="L115" s="3">
+        <v>2.52</v>
+      </c>
+      <c r="M115" s="3">
+        <v>2.44</v>
+      </c>
+      <c r="N115" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>10.46</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>9.25</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>11.08</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>9.7799999999999994</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>9.74</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>10.49</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>9.92</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>10.48</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>10.87</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>9.5</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>9.34</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>9.52</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>12.11</v>
       </c>
     </row>
@@ -47946,29 +47990,29 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -53048,134 +53092,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="6" t="s">
-        <v>15</v>
+      <c r="A113" s="6">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>0.16</v>
+        <v>3.37</v>
       </c>
       <c r="C113" s="3">
-        <v>0.08</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0.11</v>
+        <v>1.97</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>0.05</v>
+        <v>1.47</v>
       </c>
       <c r="F113" s="3">
-        <v>0.16</v>
+        <v>1.61</v>
       </c>
       <c r="G113" s="3">
-        <v>0.05</v>
+        <v>1.58</v>
       </c>
       <c r="H113" s="3">
-        <v>0.2</v>
+        <v>0.99</v>
       </c>
       <c r="I113" s="3">
-        <v>0.22</v>
+        <v>0.61</v>
       </c>
       <c r="J113" s="3">
-        <v>0.05</v>
+        <v>0.64</v>
       </c>
       <c r="K113" s="3">
-        <v>0.06</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L113" s="3">
-        <v>0.08</v>
+        <v>0.92</v>
       </c>
       <c r="M113" s="3">
-        <v>0.09</v>
+        <v>1.37</v>
       </c>
       <c r="N113" s="3">
-        <v>0</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>3.84</v>
+        <v>0.16</v>
       </c>
       <c r="C114" s="3">
-        <v>3.7</v>
+        <v>0.08</v>
       </c>
       <c r="D114" s="3">
-        <v>3.92</v>
+        <v>0.11</v>
       </c>
       <c r="E114" s="3">
-        <v>3.49</v>
+        <v>0.05</v>
       </c>
       <c r="F114" s="3">
-        <v>2.89</v>
+        <v>0.16</v>
       </c>
       <c r="G114" s="3">
-        <v>3.19</v>
+        <v>0.05</v>
       </c>
       <c r="H114" s="3">
-        <v>2.83</v>
+        <v>0.2</v>
       </c>
       <c r="I114" s="3">
-        <v>3.14</v>
+        <v>0.22</v>
       </c>
       <c r="J114" s="3">
-        <v>3</v>
+        <v>0.05</v>
       </c>
       <c r="K114" s="3">
-        <v>2.96</v>
+        <v>0.06</v>
       </c>
       <c r="L114" s="3">
-        <v>2.88</v>
+        <v>0.08</v>
       </c>
       <c r="M114" s="3">
-        <v>2.75</v>
+        <v>0.09</v>
       </c>
       <c r="N114" s="3">
-        <v>2.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>3.83</v>
+      </c>
+      <c r="C115" s="3">
+        <v>3.68</v>
+      </c>
+      <c r="D115" s="3">
+        <v>3.92</v>
+      </c>
+      <c r="E115" s="3">
+        <v>3.47</v>
+      </c>
+      <c r="F115" s="3">
+        <v>2.87</v>
+      </c>
+      <c r="G115" s="3">
+        <v>3.18</v>
+      </c>
+      <c r="H115" s="3">
+        <v>2.81</v>
+      </c>
+      <c r="I115" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="J115" s="3">
+        <v>2.98</v>
+      </c>
+      <c r="K115" s="3">
+        <v>2.94</v>
+      </c>
+      <c r="L115" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="M115" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="N115" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>12.13</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>14.87</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>15.39</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>14.24</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>8.52</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>12.87</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>8.11</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>10.64</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>11.1</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>10.01</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>10.56</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>10.050000000000001</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>9.91</v>
       </c>
     </row>
@@ -53195,23 +53283,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -58250,23 +58338,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -63489,23 +63577,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -71120,23 +71208,23 @@
       <selection activeCell="A73" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -76267,23 +76355,23 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="1" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -81415,23 +81503,23 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="12"/>
+    <col min="1" max="1" width="47.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update misc figs in createfigs.R
</commit_message>
<xml_diff>
--- a/data-raw/swfwmdrainfall.xlsx
+++ b/data-raw/swfwmdrainfall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swfwmd-my.sharepoint.com/personal/erin_walters_swfwmd_state_fl_us/Documents/AprilRain25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Hydrodat\HYDRO\HCRrain\data\Manual Refresh Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{7ACEC942-7F4D-449A-8841-4606B4D19748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D26D83B-381E-48FE-A295-5155A611B635}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3952F00-D5EA-49E0-8859-1EA1856CE45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="961" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jan-usgsbsn" sheetId="1" r:id="rId1"/>
@@ -34,20 +34,20 @@
   <definedNames>
     <definedName name="ann_usgsbasin" localSheetId="12">'ann-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="apr_usgsbasin" localSheetId="3">'apr-usgsbsn'!$A$1:$N$116</definedName>
-    <definedName name="aug_usgsbasin" localSheetId="7">'aug-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="aug_usgsbasin" localSheetId="7">'aug-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="dec_usgsbasin" localSheetId="11">'dec-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="dry_usgsbasin" localSheetId="14">'dry-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="dry_usgsbasin" localSheetId="14">'dry-usgsbsn'!$A$1:$N$117</definedName>
     <definedName name="feb_usgsbasin" localSheetId="1">'feb-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="jan_usgsbasin" localSheetId="0">'jan-usgsbsn'!$A$1:$N$116</definedName>
-    <definedName name="jul_usgsbasin" localSheetId="6">'jul-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="jun_usgsbasin" localSheetId="5">'jun-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="jul_usgsbasin" localSheetId="6">'jul-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="jun_usgsbasin" localSheetId="5">'jun-usgsbsn'!$A$1:$N$116</definedName>
     <definedName name="mar_usgsbasin" localSheetId="2">'mar-usgsbsn'!$A$1:$N$116</definedName>
-    <definedName name="may_usgsbasin" localSheetId="4">'may-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="nov_usgsbasin" localSheetId="10">'nov-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="oct_usgsbasin" localSheetId="9">'oct-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="sep_usgsbasin" localSheetId="8">'sep-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="wet_usgsbasin" localSheetId="13">'wet-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="wyr_usgsbasin" localSheetId="15">'wateryear-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="may_usgsbasin" localSheetId="4">'may-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="nov_usgsbasin" localSheetId="10">'nov-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="oct_usgsbasin" localSheetId="9">'oct-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="sep_usgsbasin" localSheetId="8">'sep-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="wet_usgsbasin" localSheetId="13">'wet-usgsbsn'!$A$1:$N$116</definedName>
+    <definedName name="wyr_usgsbasin" localSheetId="15">'wateryear-usgsbsn'!$A$1:$N$117</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="34">
   <si>
     <t>January Rainfall Summary Data by USGS Drainage Basin</t>
   </si>
@@ -1035,25 +1035,25 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="44.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6225,29 +6225,29 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="45" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -11232,134 +11232,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>0.01</v>
+        <v>2.88</v>
       </c>
       <c r="C113" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0.05</v>
+        <v>3.1</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>0.04</v>
+        <v>1.32</v>
       </c>
       <c r="F113" s="3">
-        <v>0.09</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G113" s="3">
-        <v>0.08</v>
+        <v>0.6</v>
       </c>
       <c r="H113" s="3">
-        <v>0.14000000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="I113" s="3">
-        <v>0.06</v>
+        <v>0.45</v>
       </c>
       <c r="J113" s="3">
-        <v>0.01</v>
+        <v>0.93</v>
       </c>
       <c r="K113" s="3">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="L113" s="3">
-        <v>0</v>
+        <v>0.92</v>
       </c>
       <c r="M113" s="3">
-        <v>0.03</v>
+        <v>0.76</v>
       </c>
       <c r="N113" s="3">
-        <v>0</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>2.98</v>
+        <v>0.01</v>
       </c>
       <c r="C114" s="3">
-        <v>2.9</v>
+        <v>0.11</v>
       </c>
       <c r="D114" s="3">
-        <v>3.02</v>
+        <v>0.05</v>
       </c>
       <c r="E114" s="3">
-        <v>2.93</v>
+        <v>0.04</v>
       </c>
       <c r="F114" s="3">
-        <v>3.24</v>
+        <v>0.09</v>
       </c>
       <c r="G114" s="3">
-        <v>2.89</v>
+        <v>0.08</v>
       </c>
       <c r="H114" s="3">
-        <v>3.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I114" s="3">
-        <v>2.88</v>
+        <v>0.06</v>
       </c>
       <c r="J114" s="3">
-        <v>3.02</v>
+        <v>0.01</v>
       </c>
       <c r="K114" s="3">
-        <v>3.01</v>
+        <v>0</v>
       </c>
       <c r="L114" s="3">
-        <v>3.26</v>
+        <v>0</v>
       </c>
       <c r="M114" s="3">
-        <v>3.21</v>
+        <v>0.03</v>
       </c>
       <c r="N114" s="3">
-        <v>3.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>2.98</v>
+      </c>
+      <c r="C115" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="D115" s="3">
+        <v>3.02</v>
+      </c>
+      <c r="E115" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="F115" s="3">
+        <v>3.23</v>
+      </c>
+      <c r="G115" s="3">
+        <v>2.87</v>
+      </c>
+      <c r="H115" s="3">
+        <v>3.08</v>
+      </c>
+      <c r="I115" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="J115" s="3">
+        <v>3</v>
+      </c>
+      <c r="K115" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="L115" s="3">
+        <v>3.24</v>
+      </c>
+      <c r="M115" s="3">
+        <v>3.19</v>
+      </c>
+      <c r="N115" s="3">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>10.3</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>10.26</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>12.69</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>14.03</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>9.64</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>14.15</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>10.67</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>12.26</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>13.53</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>11.99</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>12.69</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>10.25</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>13.7</v>
       </c>
     </row>
@@ -11373,27 +11417,27 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -16470,134 +16514,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C113" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0.01</v>
+        <v>0.3</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F113" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.35</v>
       </c>
       <c r="G113" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="H113" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="I113" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="J113" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="K113" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="L113" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="M113" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="N113" s="3">
         <v>0.02</v>
-      </c>
-      <c r="H113" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="I113" s="3">
-        <v>0</v>
-      </c>
-      <c r="J113" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="K113" s="3">
-        <v>0</v>
-      </c>
-      <c r="L113" s="3">
-        <v>0</v>
-      </c>
-      <c r="M113" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="N113" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>2.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C114" s="3">
-        <v>1.95</v>
+        <v>0.06</v>
       </c>
       <c r="D114" s="3">
-        <v>1.97</v>
+        <v>0.01</v>
       </c>
       <c r="E114" s="3">
-        <v>1.94</v>
+        <v>0</v>
       </c>
       <c r="F114" s="3">
-        <v>1.79</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G114" s="3">
-        <v>1.82</v>
+        <v>0.02</v>
       </c>
       <c r="H114" s="3">
-        <v>1.75</v>
+        <v>0.05</v>
       </c>
       <c r="I114" s="3">
-        <v>1.78</v>
+        <v>0</v>
       </c>
       <c r="J114" s="3">
-        <v>1.88</v>
+        <v>0.02</v>
       </c>
       <c r="K114" s="3">
-        <v>1.87</v>
+        <v>0</v>
       </c>
       <c r="L114" s="3">
-        <v>1.88</v>
+        <v>0</v>
       </c>
       <c r="M114" s="3">
-        <v>1.81</v>
+        <v>0.01</v>
       </c>
       <c r="N114" s="3">
-        <v>1.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="C115" s="3">
+        <v>1.94</v>
+      </c>
+      <c r="D115" s="3">
+        <v>1.97</v>
+      </c>
+      <c r="E115" s="3">
+        <v>1.92</v>
+      </c>
+      <c r="F115" s="3">
+        <v>1.77</v>
+      </c>
+      <c r="G115" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="H115" s="3">
+        <v>1.74</v>
+      </c>
+      <c r="I115" s="3">
+        <v>1.77</v>
+      </c>
+      <c r="J115" s="3">
+        <v>1.86</v>
+      </c>
+      <c r="K115" s="3">
+        <v>1.86</v>
+      </c>
+      <c r="L115" s="3">
+        <v>1.86</v>
+      </c>
+      <c r="M115" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="N115" s="3">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>7.44</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>6.89</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>7.67</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>8.56</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>7.16</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>7.47</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>6.63</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>6.79</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>7.05</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>7.97</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>6.66</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>7.8</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>6.24</v>
       </c>
     </row>
@@ -16617,23 +16705,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -21857,23 +21945,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="53.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -27044,29 +27132,29 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="63.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -32051,134 +32139,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>16.87</v>
+        <v>27.88</v>
       </c>
       <c r="C113" s="3">
-        <v>19.09</v>
-      </c>
-      <c r="D113" s="3">
-        <v>20.04</v>
+        <v>23.97</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>18.09</v>
+        <v>25.21</v>
       </c>
       <c r="F113" s="3">
-        <v>18.18</v>
+        <v>25.25</v>
       </c>
       <c r="G113" s="3">
-        <v>18.059999999999999</v>
+        <v>25.72</v>
       </c>
       <c r="H113" s="3">
-        <v>19.05</v>
+        <v>25.27</v>
       </c>
       <c r="I113" s="3">
-        <v>19.7</v>
+        <v>24.94</v>
       </c>
       <c r="J113" s="3">
-        <v>17.3</v>
+        <v>27.18</v>
       </c>
       <c r="K113" s="3">
-        <v>16.670000000000002</v>
+        <v>27.61</v>
       </c>
       <c r="L113" s="3">
-        <v>17.7</v>
+        <v>26.04</v>
       </c>
       <c r="M113" s="3">
-        <v>20.18</v>
+        <v>29.06</v>
       </c>
       <c r="N113" s="3">
-        <v>16.989999999999998</v>
+        <v>30.27</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>29.44</v>
+        <v>16.87</v>
       </c>
       <c r="C114" s="3">
-        <v>29.95</v>
+        <v>19.09</v>
       </c>
       <c r="D114" s="3">
-        <v>31.11</v>
+        <v>20.04</v>
       </c>
       <c r="E114" s="3">
-        <v>31.3</v>
+        <v>18.09</v>
       </c>
       <c r="F114" s="3">
-        <v>30.83</v>
+        <v>18.18</v>
       </c>
       <c r="G114" s="3">
-        <v>30.88</v>
+        <v>18.059999999999999</v>
       </c>
       <c r="H114" s="3">
-        <v>31.5</v>
+        <v>19.05</v>
       </c>
       <c r="I114" s="3">
-        <v>31.1</v>
+        <v>19.7</v>
       </c>
       <c r="J114" s="3">
-        <v>31.89</v>
+        <v>17.3</v>
       </c>
       <c r="K114" s="3">
-        <v>32.909999999999997</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="L114" s="3">
-        <v>31.47</v>
+        <v>17.7</v>
       </c>
       <c r="M114" s="3">
-        <v>33.049999999999997</v>
+        <v>20.18</v>
       </c>
       <c r="N114" s="3">
-        <v>31.89</v>
+        <v>16.989999999999998</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>29.43</v>
+      </c>
+      <c r="C115" s="3">
+        <v>29.9</v>
+      </c>
+      <c r="D115" s="3">
+        <v>31.11</v>
+      </c>
+      <c r="E115" s="3">
+        <v>31.24</v>
+      </c>
+      <c r="F115" s="3">
+        <v>30.78</v>
+      </c>
+      <c r="G115" s="3">
+        <v>30.83</v>
+      </c>
+      <c r="H115" s="3">
+        <v>31.44</v>
+      </c>
+      <c r="I115" s="3">
+        <v>31.05</v>
+      </c>
+      <c r="J115" s="3">
+        <v>31.85</v>
+      </c>
+      <c r="K115" s="3">
+        <v>32.86</v>
+      </c>
+      <c r="L115" s="3">
+        <v>31.42</v>
+      </c>
+      <c r="M115" s="3">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="N115" s="3">
+        <v>31.88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>43.49</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>49.58</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>53.69</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>52.83</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>44.6</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>48.47</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>46.12</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>49.52</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>50.91</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>52.67</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>51.41</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>57.15</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>59.25</v>
       </c>
     </row>
@@ -32192,29 +32324,29 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:P116"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="59.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -37297,174 +37429,218 @@
         <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>17.23</v>
+        <v>21.3</v>
       </c>
       <c r="C113" s="3">
-        <v>17.66</v>
+        <v>23.01</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>21.73</v>
+        <v>26.41</v>
       </c>
       <c r="F113" s="3">
-        <v>13.94</v>
+        <v>23.41</v>
       </c>
       <c r="G113" s="3">
-        <v>21.87</v>
+        <v>25.88</v>
       </c>
       <c r="H113" s="3">
-        <v>12.59</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="I113" s="3">
-        <v>15.53</v>
+        <v>21.3</v>
       </c>
       <c r="J113" s="3">
-        <v>14.56</v>
+        <v>19.47</v>
       </c>
       <c r="K113" s="3">
-        <v>13.04</v>
+        <v>16.93</v>
       </c>
       <c r="L113" s="3">
-        <v>13.71</v>
+        <v>17.04</v>
       </c>
       <c r="M113" s="3">
-        <v>13.19</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="N113" s="3">
-        <v>12.84</v>
+        <v>16.309999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B114" s="3">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="C114" s="3">
-        <v>10.92</v>
-      </c>
-      <c r="D114" s="3">
-        <v>1.84</v>
-      </c>
-      <c r="E114" s="3">
-        <v>10.29</v>
-      </c>
-      <c r="F114" s="3">
-        <v>9.16</v>
-      </c>
-      <c r="G114" s="3">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="H114" s="3">
-        <v>9.82</v>
-      </c>
-      <c r="I114" s="3">
-        <v>10.46</v>
-      </c>
-      <c r="J114" s="3">
-        <v>9.5399999999999991</v>
-      </c>
-      <c r="K114" s="3">
-        <v>9.31</v>
-      </c>
-      <c r="L114" s="3">
-        <v>7.85</v>
-      </c>
-      <c r="M114" s="3">
-        <v>6.64</v>
-      </c>
-      <c r="N114" s="3">
-        <v>6.25</v>
+      <c r="A114" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B115" s="3">
-        <v>24.54</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="C115" s="3">
-        <v>22.85</v>
+        <v>10.92</v>
       </c>
       <c r="D115" s="3">
-        <v>22.99</v>
+        <v>1.84</v>
       </c>
       <c r="E115" s="3">
-        <v>22.34</v>
+        <v>10.29</v>
       </c>
       <c r="F115" s="3">
-        <v>20.97</v>
+        <v>9.16</v>
       </c>
       <c r="G115" s="3">
-        <v>20.74</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="H115" s="3">
-        <v>20.48</v>
+        <v>9.82</v>
       </c>
       <c r="I115" s="3">
-        <v>21.36</v>
+        <v>10.46</v>
       </c>
       <c r="J115" s="3">
-        <v>20.89</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="K115" s="3">
-        <v>20.47</v>
+        <v>9.31</v>
       </c>
       <c r="L115" s="3">
-        <v>20.12</v>
+        <v>7.85</v>
       </c>
       <c r="M115" s="3">
-        <v>20.03</v>
+        <v>6.64</v>
       </c>
       <c r="N115" s="3">
-        <v>19.32</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="3">
+        <v>24.58</v>
+      </c>
+      <c r="C116" s="3">
+        <v>22.9</v>
+      </c>
+      <c r="D116" s="3">
+        <v>22.99</v>
+      </c>
+      <c r="E116" s="3">
+        <v>22.38</v>
+      </c>
+      <c r="F116" s="3">
+        <v>21.06</v>
+      </c>
+      <c r="G116" s="3">
+        <v>20.78</v>
+      </c>
+      <c r="H116" s="3">
+        <v>20.54</v>
+      </c>
+      <c r="I116" s="3">
+        <v>21.42</v>
+      </c>
+      <c r="J116" s="3">
+        <v>20.94</v>
+      </c>
+      <c r="K116" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="L116" s="3">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="M116" s="3">
+        <v>20.07</v>
+      </c>
+      <c r="N116" s="3">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B116" s="3">
+      <c r="B117" s="3">
         <v>49.2</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C117" s="3">
         <v>43.06</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D117" s="3">
         <v>47.23</v>
       </c>
-      <c r="E116" s="3">
+      <c r="E117" s="3">
         <v>44.34</v>
       </c>
-      <c r="F116" s="3">
+      <c r="F117" s="3">
         <v>38.200000000000003</v>
       </c>
-      <c r="G116" s="3">
+      <c r="G117" s="3">
         <v>46.66</v>
       </c>
-      <c r="H116" s="3">
+      <c r="H117" s="3">
         <v>38.880000000000003</v>
       </c>
-      <c r="I116" s="3">
+      <c r="I117" s="3">
         <v>43.59</v>
       </c>
-      <c r="J116" s="3">
+      <c r="J117" s="3">
         <v>44.67</v>
       </c>
-      <c r="K116" s="3">
+      <c r="K117" s="3">
         <v>45.5</v>
       </c>
-      <c r="L116" s="3">
+      <c r="L117" s="3">
         <v>44.06</v>
       </c>
-      <c r="M116" s="3">
+      <c r="M117" s="3">
         <v>42.03</v>
       </c>
-      <c r="N116" s="3">
+      <c r="N117" s="3">
         <v>36.36</v>
       </c>
     </row>
@@ -37478,29 +37654,29 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:P117"/>
+  <dimension ref="A1:P118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="65.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -42584,192 +42760,236 @@
       <c r="A113" s="2">
         <v>2025</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>33</v>
+      <c r="B113" s="3">
+        <v>49.18</v>
+      </c>
+      <c r="C113" s="3">
+        <v>46.98</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E113" s="3">
+        <v>51.62</v>
+      </c>
+      <c r="F113" s="3">
+        <v>48.66</v>
+      </c>
+      <c r="G113" s="3">
+        <v>51.6</v>
+      </c>
+      <c r="H113" s="3">
+        <v>44.26</v>
+      </c>
+      <c r="I113" s="3">
+        <v>46.24</v>
+      </c>
+      <c r="J113" s="3">
+        <v>46.65</v>
+      </c>
+      <c r="K113" s="3">
+        <v>44.54</v>
+      </c>
+      <c r="L113" s="3">
+        <v>43.08</v>
+      </c>
+      <c r="M113" s="3">
+        <v>45.66</v>
+      </c>
+      <c r="N113" s="3">
+        <v>46.58</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F113" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G113" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H113" s="3" t="s">
+      <c r="E114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I113" s="3" t="s">
+      <c r="F114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J113" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K113" s="3" t="s">
+      <c r="H114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L113" s="3" t="s">
+      <c r="I114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M113" s="3" t="s">
+      <c r="J114" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N113" s="3" t="s">
+      <c r="K114" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B114" s="3">
-        <v>34.46</v>
-      </c>
-      <c r="C114" s="3">
-        <v>36.869999999999997</v>
-      </c>
-      <c r="D114" s="3">
-        <v>38.14</v>
-      </c>
-      <c r="E114" s="3">
-        <v>35.57</v>
-      </c>
-      <c r="F114" s="3">
-        <v>34.97</v>
-      </c>
-      <c r="G114" s="3">
-        <v>33.29</v>
-      </c>
-      <c r="H114" s="3">
-        <v>36.57</v>
-      </c>
-      <c r="I114" s="3">
-        <v>37.61</v>
-      </c>
-      <c r="J114" s="3">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="K114" s="3">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="L114" s="3">
-        <v>31.42</v>
-      </c>
-      <c r="M114" s="3">
-        <v>35.54</v>
-      </c>
-      <c r="N114" s="3">
-        <v>30.04</v>
+      <c r="L114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B115" s="3">
-        <v>54.23</v>
+        <v>34.46</v>
       </c>
       <c r="C115" s="3">
-        <v>52.99</v>
+        <v>36.869999999999997</v>
       </c>
       <c r="D115" s="3">
-        <v>54.5</v>
+        <v>38.14</v>
       </c>
       <c r="E115" s="3">
-        <v>53.79</v>
+        <v>35.57</v>
       </c>
       <c r="F115" s="3">
-        <v>51.88</v>
+        <v>34.97</v>
       </c>
       <c r="G115" s="3">
-        <v>51.69</v>
+        <v>33.29</v>
       </c>
       <c r="H115" s="3">
-        <v>52.11</v>
+        <v>36.57</v>
       </c>
       <c r="I115" s="3">
-        <v>52.63</v>
+        <v>37.61</v>
       </c>
       <c r="J115" s="3">
-        <v>52.9</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="K115" s="3">
-        <v>53.5</v>
+        <v>34.479999999999997</v>
       </c>
       <c r="L115" s="3">
-        <v>51.71</v>
+        <v>31.42</v>
       </c>
       <c r="M115" s="3">
-        <v>53.24</v>
+        <v>35.54</v>
       </c>
       <c r="N115" s="3">
-        <v>51.37</v>
+        <v>30.04</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="3">
+        <v>54.18</v>
+      </c>
+      <c r="C116" s="3">
+        <v>52.94</v>
+      </c>
+      <c r="D116" s="3">
+        <v>54.5</v>
+      </c>
+      <c r="E116" s="3">
+        <v>53.77</v>
+      </c>
+      <c r="F116" s="3">
+        <v>51.85</v>
+      </c>
+      <c r="G116" s="3">
+        <v>51.68</v>
+      </c>
+      <c r="H116" s="3">
+        <v>52.04</v>
+      </c>
+      <c r="I116" s="3">
+        <v>52.57</v>
+      </c>
+      <c r="J116" s="3">
+        <v>52.84</v>
+      </c>
+      <c r="K116" s="3">
+        <v>53.42</v>
+      </c>
+      <c r="L116" s="3">
+        <v>51.63</v>
+      </c>
+      <c r="M116" s="3">
+        <v>53.17</v>
+      </c>
+      <c r="N116" s="3">
+        <v>51.33</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B116" s="3">
+      <c r="B117" s="3">
         <v>81.92</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C117" s="3">
         <v>79.400000000000006</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D117" s="3">
         <v>82.49</v>
       </c>
-      <c r="E116" s="3">
+      <c r="E117" s="3">
         <v>78.349999999999994</v>
       </c>
-      <c r="F116" s="3">
+      <c r="F117" s="3">
         <v>74.44</v>
       </c>
-      <c r="G116" s="3">
+      <c r="G117" s="3">
         <v>82.75</v>
       </c>
-      <c r="H116" s="3">
+      <c r="H117" s="3">
         <v>74.23</v>
       </c>
-      <c r="I116" s="3">
+      <c r="I117" s="3">
         <v>77.78</v>
       </c>
-      <c r="J116" s="3">
+      <c r="J117" s="3">
         <v>83.68</v>
       </c>
-      <c r="K116" s="3">
+      <c r="K117" s="3">
         <v>88.93</v>
       </c>
-      <c r="L116" s="3">
+      <c r="L117" s="3">
         <v>85.26</v>
       </c>
-      <c r="M116" s="3">
+      <c r="M117" s="3">
         <v>80.010000000000005</v>
       </c>
-      <c r="N116" s="3">
+      <c r="N117" s="3">
         <v>86.76</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-      <c r="J117" s="3"/>
-      <c r="K117" s="3"/>
-      <c r="L117" s="3"/>
-      <c r="M117" s="3"/>
-      <c r="N117" s="3"/>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -42784,7 +43004,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -42800,23 +43020,23 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="6.44140625" style="1"/>
+    <col min="1" max="1" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="6.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -47994,23 +48214,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -53281,23 +53501,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -58374,29 +58594,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -63473,134 +63693,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>0.22</v>
+        <v>4.07</v>
       </c>
       <c r="C113" s="3">
-        <v>0.49</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0.27</v>
+        <v>5.35</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>0.2</v>
+        <v>4.68</v>
       </c>
       <c r="F113" s="3">
-        <v>0.62</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="G113" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>4.01</v>
       </c>
       <c r="H113" s="3">
-        <v>0.28000000000000003</v>
+        <v>6.4</v>
       </c>
       <c r="I113" s="3">
-        <v>0.47</v>
+        <v>5.77</v>
       </c>
       <c r="J113" s="3">
-        <v>0.1</v>
+        <v>4.91</v>
       </c>
       <c r="K113" s="3">
-        <v>0.05</v>
+        <v>3.89</v>
       </c>
       <c r="L113" s="3">
-        <v>0.17</v>
+        <v>3.33</v>
       </c>
       <c r="M113" s="3">
-        <v>0.34</v>
+        <v>3.41</v>
       </c>
       <c r="N113" s="3">
-        <v>0.01</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>3.54</v>
+        <v>0.22</v>
       </c>
       <c r="C114" s="3">
-        <v>3.79</v>
+        <v>0.49</v>
       </c>
       <c r="D114" s="3">
-        <v>3.41</v>
+        <v>0.27</v>
       </c>
       <c r="E114" s="3">
-        <v>3.78</v>
+        <v>0.2</v>
       </c>
       <c r="F114" s="3">
-        <v>4.1100000000000003</v>
+        <v>0.62</v>
       </c>
       <c r="G114" s="3">
-        <v>3.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H114" s="3">
-        <v>3.96</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I114" s="3">
-        <v>3.89</v>
+        <v>0.47</v>
       </c>
       <c r="J114" s="3">
-        <v>3.42</v>
+        <v>0.1</v>
       </c>
       <c r="K114" s="3">
-        <v>3.16</v>
+        <v>0.05</v>
       </c>
       <c r="L114" s="3">
-        <v>2.96</v>
+        <v>0.17</v>
       </c>
       <c r="M114" s="3">
-        <v>3.41</v>
+        <v>0.34</v>
       </c>
       <c r="N114" s="3">
-        <v>3.35</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>3.54</v>
+      </c>
+      <c r="C115" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="D115" s="3">
+        <v>3.41</v>
+      </c>
+      <c r="E115" s="3">
+        <v>3.79</v>
+      </c>
+      <c r="F115" s="3">
+        <v>4.16</v>
+      </c>
+      <c r="G115" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="H115" s="3">
+        <v>3.98</v>
+      </c>
+      <c r="I115" s="3">
+        <v>3.91</v>
+      </c>
+      <c r="J115" s="3">
+        <v>3.43</v>
+      </c>
+      <c r="K115" s="3">
+        <v>3.17</v>
+      </c>
+      <c r="L115" s="3">
+        <v>2.96</v>
+      </c>
+      <c r="M115" s="3">
+        <v>3.41</v>
+      </c>
+      <c r="N115" s="3">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>11.69</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>12.26</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>13.35</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>13.57</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>12.14</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>12.46</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>12.43</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>14.28</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>11.26</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>10.88</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>10.52</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>13.41</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>13.46</v>
       </c>
     </row>
@@ -63613,29 +63877,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AP115"/>
+  <dimension ref="A1:AP116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -71104,134 +71368,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>1.46</v>
+        <v>7.39</v>
       </c>
       <c r="C113" s="3">
-        <v>1.35</v>
-      </c>
-      <c r="D113" s="3">
-        <v>1.36</v>
+        <v>5.91</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>1.82</v>
+        <v>7.02</v>
       </c>
       <c r="F113" s="3">
-        <v>1.49</v>
+        <v>6.49</v>
       </c>
       <c r="G113" s="3">
-        <v>1.61</v>
+        <v>7.16</v>
       </c>
       <c r="H113" s="3">
-        <v>2.52</v>
+        <v>7.58</v>
       </c>
       <c r="I113" s="3">
-        <v>2.5499999999999998</v>
+        <v>7.32</v>
       </c>
       <c r="J113" s="3">
-        <v>2.06</v>
+        <v>8.99</v>
       </c>
       <c r="K113" s="3">
-        <v>1.3</v>
+        <v>9.69</v>
       </c>
       <c r="L113" s="3">
-        <v>2.02</v>
+        <v>9.51</v>
       </c>
       <c r="M113" s="3">
-        <v>2.2400000000000002</v>
+        <v>10.6</v>
       </c>
       <c r="N113" s="3">
-        <v>0</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>7.18</v>
+        <v>1.46</v>
       </c>
       <c r="C114" s="3">
-        <v>7.71</v>
+        <v>1.35</v>
       </c>
       <c r="D114" s="3">
-        <v>7.04</v>
+        <v>1.36</v>
       </c>
       <c r="E114" s="3">
-        <v>7.89</v>
+        <v>1.82</v>
       </c>
       <c r="F114" s="3">
-        <v>8.1999999999999993</v>
+        <v>1.49</v>
       </c>
       <c r="G114" s="3">
-        <v>6.89</v>
+        <v>1.61</v>
       </c>
       <c r="H114" s="3">
-        <v>8.33</v>
+        <v>2.52</v>
       </c>
       <c r="I114" s="3">
-        <v>7.9</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="J114" s="3">
-        <v>7.6</v>
+        <v>2.06</v>
       </c>
       <c r="K114" s="3">
-        <v>7.5</v>
+        <v>1.3</v>
       </c>
       <c r="L114" s="3">
-        <v>7.14</v>
+        <v>2.02</v>
       </c>
       <c r="M114" s="3">
-        <v>8.2200000000000006</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="N114" s="3">
-        <v>8.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>7.18</v>
+      </c>
+      <c r="C115" s="3">
+        <v>7.69</v>
+      </c>
+      <c r="D115" s="3">
+        <v>7.04</v>
+      </c>
+      <c r="E115" s="3">
+        <v>7.88</v>
+      </c>
+      <c r="F115" s="3">
+        <v>8.18</v>
+      </c>
+      <c r="G115" s="3">
+        <v>6.89</v>
+      </c>
+      <c r="H115" s="3">
+        <v>8.33</v>
+      </c>
+      <c r="I115" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="J115" s="3">
+        <v>7.61</v>
+      </c>
+      <c r="K115" s="3">
+        <v>7.52</v>
+      </c>
+      <c r="L115" s="3">
+        <v>7.16</v>
+      </c>
+      <c r="M115" s="3">
+        <v>8.24</v>
+      </c>
+      <c r="N115" s="3">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>14.32</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>16.21</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>17.989999999999998</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>18.91</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>16.03</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>18.59</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>17.16</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>16.059999999999999</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>16.95</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>21.8</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>21.44</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>22.25</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>24.62</v>
       </c>
     </row>
@@ -71244,29 +71552,29 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A73" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -76251,134 +76559,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+      <c r="A113" s="2">
+        <v>2025</v>
       </c>
       <c r="B113" s="3">
-        <v>3.26</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="C113" s="3">
-        <v>3.54</v>
-      </c>
-      <c r="D113" s="3">
-        <v>3.63</v>
+        <v>7</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="3">
-        <v>3.66</v>
+        <v>6.81</v>
       </c>
       <c r="F113" s="3">
-        <v>3.58</v>
+        <v>7.3</v>
       </c>
       <c r="G113" s="3">
-        <v>2.86</v>
+        <v>6.89</v>
       </c>
       <c r="H113" s="3">
-        <v>2.96</v>
+        <v>6.78</v>
       </c>
       <c r="I113" s="3">
-        <v>3.68</v>
+        <v>5.17</v>
       </c>
       <c r="J113" s="3">
-        <v>3.05</v>
+        <v>6.32</v>
       </c>
       <c r="K113" s="3">
-        <v>2.82</v>
+        <v>6.48</v>
       </c>
       <c r="L113" s="3">
-        <v>2.62</v>
+        <v>5.24</v>
       </c>
       <c r="M113" s="3">
-        <v>2.41</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="N113" s="3">
-        <v>1.75</v>
+        <v>7.66</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3">
-        <v>8.07</v>
+        <v>3.26</v>
       </c>
       <c r="C114" s="3">
-        <v>8.1199999999999992</v>
+        <v>3.54</v>
       </c>
       <c r="D114" s="3">
-        <v>8.7200000000000006</v>
+        <v>3.63</v>
       </c>
       <c r="E114" s="3">
-        <v>8.31</v>
+        <v>3.66</v>
       </c>
       <c r="F114" s="3">
-        <v>7.92</v>
+        <v>3.58</v>
       </c>
       <c r="G114" s="3">
-        <v>8.4</v>
+        <v>2.86</v>
       </c>
       <c r="H114" s="3">
-        <v>8.0299999999999994</v>
+        <v>2.96</v>
       </c>
       <c r="I114" s="3">
-        <v>8.16</v>
+        <v>3.68</v>
       </c>
       <c r="J114" s="3">
-        <v>8.4499999999999993</v>
+        <v>3.05</v>
       </c>
       <c r="K114" s="3">
-        <v>8.67</v>
+        <v>2.82</v>
       </c>
       <c r="L114" s="3">
-        <v>7.96</v>
+        <v>2.62</v>
       </c>
       <c r="M114" s="3">
-        <v>8.3800000000000008</v>
+        <v>2.41</v>
       </c>
       <c r="N114" s="3">
-        <v>7.73</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="3">
+        <v>8.08</v>
+      </c>
+      <c r="C115" s="3">
+        <v>8.11</v>
+      </c>
+      <c r="D115" s="3">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="E115" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F115" s="3">
+        <v>7.91</v>
+      </c>
+      <c r="G115" s="3">
+        <v>8.39</v>
+      </c>
+      <c r="H115" s="3">
+        <v>8.02</v>
+      </c>
+      <c r="I115" s="3">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="J115" s="3">
+        <v>8.43</v>
+      </c>
+      <c r="K115" s="3">
+        <v>8.65</v>
+      </c>
+      <c r="L115" s="3">
+        <v>7.94</v>
+      </c>
+      <c r="M115" s="3">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="N115" s="3">
+        <v>7.73</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B116" s="3">
         <v>14.37</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C116" s="3">
         <v>14.74</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>16.809999999999999</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>16.350000000000001</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>15.78</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>19.88</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>13.56</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>18.09</v>
       </c>
-      <c r="J115" s="3">
+      <c r="J116" s="3">
         <v>18.170000000000002</v>
       </c>
-      <c r="K115" s="3">
+      <c r="K116" s="3">
         <v>20.82</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L116" s="3">
         <v>16.7</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M116" s="3">
         <v>16.2</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N116" s="3">
         <v>18.25</v>
       </c>
     </row>
@@ -76391,29 +76743,29 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="1" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -81398,134 +81750,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
-        <v>15</v>
+      <c r="A113" s="7">
+        <v>2025</v>
       </c>
       <c r="B113" s="8">
-        <v>2.4500000000000002</v>
+        <v>6.17</v>
       </c>
       <c r="C113" s="8">
-        <v>2.44</v>
-      </c>
-      <c r="D113" s="8">
-        <v>3.52</v>
+        <v>7.38</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="8">
-        <v>3.09</v>
+        <v>8.39</v>
       </c>
       <c r="F113" s="8">
-        <v>3.21</v>
+        <v>7.22</v>
       </c>
       <c r="G113" s="8">
-        <v>2.12</v>
+        <v>9.73</v>
       </c>
       <c r="H113" s="8">
-        <v>3.37</v>
+        <v>6.56</v>
       </c>
       <c r="I113" s="8">
-        <v>3.68</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J113" s="8">
-        <v>2.98</v>
+        <v>9.15</v>
       </c>
       <c r="K113" s="8">
-        <v>2.54</v>
+        <v>9.3699999999999992</v>
       </c>
       <c r="L113" s="8">
-        <v>2.4</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="M113" s="8">
-        <v>2.52</v>
+        <v>7.61</v>
       </c>
       <c r="N113" s="8">
-        <v>1.86</v>
+        <v>8.7100000000000009</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="8">
-        <v>8.09</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="C114" s="8">
-        <v>7.82</v>
+        <v>2.44</v>
       </c>
       <c r="D114" s="8">
-        <v>8.51</v>
+        <v>3.52</v>
       </c>
       <c r="E114" s="8">
-        <v>8.2899999999999991</v>
+        <v>3.09</v>
       </c>
       <c r="F114" s="8">
-        <v>7.56</v>
+        <v>3.21</v>
       </c>
       <c r="G114" s="8">
-        <v>8.69</v>
+        <v>2.12</v>
       </c>
       <c r="H114" s="8">
-        <v>7.75</v>
+        <v>3.37</v>
       </c>
       <c r="I114" s="8">
-        <v>8.1300000000000008</v>
+        <v>3.68</v>
       </c>
       <c r="J114" s="8">
-        <v>8.6</v>
+        <v>2.98</v>
       </c>
       <c r="K114" s="8">
-        <v>9.1999999999999993</v>
+        <v>2.54</v>
       </c>
       <c r="L114" s="8">
-        <v>8.68</v>
+        <v>2.4</v>
       </c>
       <c r="M114" s="8">
-        <v>8.67</v>
+        <v>2.52</v>
       </c>
       <c r="N114" s="8">
-        <v>8.14</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="8">
+        <v>8.08</v>
+      </c>
+      <c r="C115" s="8">
+        <v>7.81</v>
+      </c>
+      <c r="D115" s="8">
+        <v>8.51</v>
+      </c>
+      <c r="E115" s="8">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="F115" s="8">
+        <v>7.56</v>
+      </c>
+      <c r="G115" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H115" s="8">
+        <v>7.73</v>
+      </c>
+      <c r="I115" s="8">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="J115" s="8">
+        <v>8.6</v>
+      </c>
+      <c r="K115" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L115" s="8">
+        <v>8.68</v>
+      </c>
+      <c r="M115" s="8">
+        <v>8.66</v>
+      </c>
+      <c r="N115" s="8">
+        <v>8.14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="8">
+      <c r="B116" s="8">
         <v>15.35</v>
       </c>
-      <c r="C115" s="8">
+      <c r="C116" s="8">
         <v>15.27</v>
       </c>
-      <c r="D115" s="8">
+      <c r="D116" s="8">
         <v>20.3</v>
       </c>
-      <c r="E115" s="8">
+      <c r="E116" s="8">
         <v>15.9</v>
       </c>
-      <c r="F115" s="8">
+      <c r="F116" s="8">
         <v>15.78</v>
       </c>
-      <c r="G115" s="8">
+      <c r="G116" s="8">
         <v>19.829999999999998</v>
       </c>
-      <c r="H115" s="8">
+      <c r="H116" s="8">
         <v>15.9</v>
       </c>
-      <c r="I115" s="8">
+      <c r="I116" s="8">
         <v>15.34</v>
       </c>
-      <c r="J115" s="8">
+      <c r="J116" s="8">
         <v>18.02</v>
       </c>
-      <c r="K115" s="8">
+      <c r="K116" s="8">
         <v>20.76</v>
       </c>
-      <c r="L115" s="8">
+      <c r="L116" s="8">
         <v>19.440000000000001</v>
       </c>
-      <c r="M115" s="8">
+      <c r="M116" s="8">
         <v>18.14</v>
       </c>
-      <c r="N115" s="8">
+      <c r="N116" s="8">
         <v>19.559999999999999</v>
       </c>
     </row>
@@ -81539,29 +81935,29 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="12"/>
+    <col min="1" max="1" width="47.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -86546,134 +86942,178 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="10" t="s">
-        <v>15</v>
+      <c r="A113" s="10">
+        <v>2025</v>
       </c>
       <c r="B113" s="11">
-        <v>0.73</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="C113" s="11">
-        <v>1.19</v>
-      </c>
-      <c r="D113" s="11">
-        <v>0.77</v>
+        <v>3.68</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="E113" s="11">
-        <v>0.92</v>
+        <v>2.99</v>
       </c>
       <c r="F113" s="11">
-        <v>1.2</v>
+        <v>4.24</v>
       </c>
       <c r="G113" s="11">
-        <v>1.65</v>
+        <v>1.94</v>
       </c>
       <c r="H113" s="11">
-        <v>1.83</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="I113" s="11">
-        <v>0.89</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="J113" s="11">
-        <v>1.21</v>
+        <v>2.72</v>
       </c>
       <c r="K113" s="11">
-        <v>1.61</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="L113" s="11">
-        <v>1.59</v>
+        <v>2.09</v>
       </c>
       <c r="M113" s="11">
-        <v>1.7</v>
+        <v>2.73</v>
       </c>
       <c r="N113" s="11">
-        <v>1.92</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="11">
-        <v>6.1</v>
+        <v>0.73</v>
       </c>
       <c r="C114" s="11">
-        <v>6.3</v>
+        <v>1.19</v>
       </c>
       <c r="D114" s="11">
-        <v>6.83</v>
+        <v>0.77</v>
       </c>
       <c r="E114" s="11">
-        <v>6.8</v>
+        <v>0.92</v>
       </c>
       <c r="F114" s="11">
-        <v>7.14</v>
+        <v>1.2</v>
       </c>
       <c r="G114" s="11">
-        <v>6.9</v>
+        <v>1.65</v>
       </c>
       <c r="H114" s="11">
-        <v>7.4</v>
+        <v>1.83</v>
       </c>
       <c r="I114" s="11">
-        <v>6.91</v>
+        <v>0.89</v>
       </c>
       <c r="J114" s="11">
-        <v>7.24</v>
+        <v>1.21</v>
       </c>
       <c r="K114" s="11">
-        <v>7.54</v>
+        <v>1.61</v>
       </c>
       <c r="L114" s="11">
-        <v>7.7</v>
+        <v>1.59</v>
       </c>
       <c r="M114" s="11">
-        <v>7.78</v>
+        <v>1.7</v>
       </c>
       <c r="N114" s="11">
-        <v>7.96</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="11">
+        <v>6.09</v>
+      </c>
+      <c r="C115" s="11">
+        <v>6.28</v>
+      </c>
+      <c r="D115" s="11">
+        <v>6.83</v>
+      </c>
+      <c r="E115" s="11">
+        <v>6.77</v>
+      </c>
+      <c r="F115" s="11">
+        <v>7.12</v>
+      </c>
+      <c r="G115" s="11">
+        <v>6.85</v>
+      </c>
+      <c r="H115" s="11">
+        <v>7.37</v>
+      </c>
+      <c r="I115" s="11">
+        <v>6.88</v>
+      </c>
+      <c r="J115" s="11">
+        <v>7.2</v>
+      </c>
+      <c r="K115" s="11">
+        <v>7.49</v>
+      </c>
+      <c r="L115" s="11">
+        <v>7.65</v>
+      </c>
+      <c r="M115" s="11">
+        <v>7.74</v>
+      </c>
+      <c r="N115" s="11">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="11">
+      <c r="B116" s="11">
         <v>18.28</v>
       </c>
-      <c r="C115" s="11">
+      <c r="C116" s="11">
         <v>16.48</v>
       </c>
-      <c r="D115" s="11">
+      <c r="D116" s="11">
         <v>17.46</v>
       </c>
-      <c r="E115" s="11">
+      <c r="E116" s="11">
         <v>16.14</v>
       </c>
-      <c r="F115" s="11">
+      <c r="F116" s="11">
         <v>21.47</v>
       </c>
-      <c r="G115" s="11">
+      <c r="G116" s="11">
         <v>16.53</v>
       </c>
-      <c r="H115" s="11">
+      <c r="H116" s="11">
         <v>21.77</v>
       </c>
-      <c r="I115" s="11">
+      <c r="I116" s="11">
         <v>15.64</v>
       </c>
-      <c r="J115" s="11">
+      <c r="J116" s="11">
         <v>16.100000000000001</v>
       </c>
-      <c r="K115" s="11">
+      <c r="K116" s="11">
         <v>17.27</v>
       </c>
-      <c r="L115" s="11">
+      <c r="L116" s="11">
         <v>18.18</v>
       </c>
-      <c r="M115" s="11">
+      <c r="M116" s="11">
         <v>25.66</v>
       </c>
-      <c r="N115" s="11">
+      <c r="N116" s="11">
         <v>22.57</v>
       </c>
     </row>

</xml_diff>